<commit_message>
Add wikidata.json, find absent translations
</commit_message>
<xml_diff>
--- a/hpo_translator/hpo_translation.xlsx
+++ b/hpo_translator/hpo_translation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -25,34 +25,172 @@
     <t>spanish</t>
   </si>
   <si>
-    <t>HP:0045052</t>
-  </si>
-  <si>
-    <t>HP:0045054</t>
-  </si>
-  <si>
-    <t>Abnormality of the brachial nerve plexus</t>
-  </si>
-  <si>
-    <t>Any abnormality of the brachial nerve plexus.</t>
-  </si>
-  <si>
-    <t>Brachial plexus neuropathy</t>
-  </si>
-  <si>
-    <t>Related to ticket: https://github.com/obophenotype/human-phenotype-ontology/issues/484</t>
-  </si>
-  <si>
-    <t>Anomalía del plexo braquial.</t>
-  </si>
-  <si>
-    <t>Cualquier anomalía del plexo braquial.</t>
-  </si>
-  <si>
-    <t>Neuropatía del plexo braquial.</t>
-  </si>
-  <si>
-    <t>Related to ticket: https://github.com/obophenotype/human-fenotype-onthology/thisures/484</t>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>HP:0040279</t>
+  </si>
+  <si>
+    <t>HP:0040280</t>
+  </si>
+  <si>
+    <t>HP:0040281</t>
+  </si>
+  <si>
+    <t>HP:0040282</t>
+  </si>
+  <si>
+    <t>HP:0040283</t>
+  </si>
+  <si>
+    <t>HP:0040284</t>
+  </si>
+  <si>
+    <t>HP:0040285</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Class to represent frequency of phenotypic abnormalities within a patient cohort.</t>
+  </si>
+  <si>
+    <t>Aligned with Orphanet</t>
+  </si>
+  <si>
+    <t>Obligate</t>
+  </si>
+  <si>
+    <t>Always present, i.e. in 100% of the cases.</t>
+  </si>
+  <si>
+    <t>Obligate (100%)</t>
+  </si>
+  <si>
+    <t>Very frequent</t>
+  </si>
+  <si>
+    <t>Present in 80% to 99% of the cases.</t>
+  </si>
+  <si>
+    <t>Very frequent (99-80%)</t>
+  </si>
+  <si>
+    <t>Frequent</t>
+  </si>
+  <si>
+    <t>Present in 30% to 79% of the cases.</t>
+  </si>
+  <si>
+    <t>Frequent (79-30%)</t>
+  </si>
+  <si>
+    <t>Occasional</t>
+  </si>
+  <si>
+    <t>Present in 5% to 29% of the cases.</t>
+  </si>
+  <si>
+    <t>Occasional (29-5%)</t>
+  </si>
+  <si>
+    <t>Very rare</t>
+  </si>
+  <si>
+    <t>Present in 1% to 4% of the cases.</t>
+  </si>
+  <si>
+    <t>Very rare (&amp;lt;4-1%)</t>
+  </si>
+  <si>
+    <t>Very rare (&lt;4-1%)</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>Present in 0% of the cases.</t>
+  </si>
+  <si>
+    <t>Excluded (0%)</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>Clase para representar la frecuencia de anomalías fenotípicas dentro de una cohorte de pacientes.</t>
+  </si>
+  <si>
+    <t>Concordante con Orphanet</t>
+  </si>
+  <si>
+    <t>Obligado</t>
+  </si>
+  <si>
+    <t>Siempre presente, es decir, en el 100% de los casos.</t>
+  </si>
+  <si>
+    <t>Obligado (100%)</t>
+  </si>
+  <si>
+    <t>Muy frecuente</t>
+  </si>
+  <si>
+    <t>Presentar en 80-99% de los casos.</t>
+  </si>
+  <si>
+    <t>Muy frecuente (99-80%)</t>
+  </si>
+  <si>
+    <t>Frecuente</t>
+  </si>
+  <si>
+    <t>Presente en 30% a 79% de los casos.</t>
+  </si>
+  <si>
+    <t>Frecuente (79-30%)</t>
+  </si>
+  <si>
+    <t>Ocasional</t>
+  </si>
+  <si>
+    <t>Presente en 5% a 29% de los casos.</t>
+  </si>
+  <si>
+    <t>Ocasional (29-5%)</t>
+  </si>
+  <si>
+    <t>Muy raro</t>
+  </si>
+  <si>
+    <t>Presente en 1% a 4% de los casos.</t>
+  </si>
+  <si>
+    <t>Muy raro (&amp;lt;4-1%)</t>
+  </si>
+  <si>
+    <t>Muy raro (&lt;4-1%)</t>
+  </si>
+  <si>
+    <t>Excluido</t>
+  </si>
+  <si>
+    <t>Presente en 0% de los casos.</t>
+  </si>
+  <si>
+    <t>Excluido (0%)</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>synonym</t>
   </si>
 </sst>
 </file>
@@ -105,12 +243,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:D23" totalsRowShown="0">
+  <autoFilter ref="A1:D23"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="id" dataDxfId="0"/>
     <tableColumn id="2" name="english" dataDxfId="0"/>
     <tableColumn id="3" name="spanish" dataDxfId="0"/>
+    <tableColumn id="4" name="kind" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -401,18 +540,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,49 +562,316 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>